<commit_message>
working for copy-paste 3 plaste input
</commit_message>
<xml_diff>
--- a/data/mapping1.xlsx
+++ b/data/mapping1.xlsx
@@ -1,36 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyoungblut/dev/R/plateReaderShiny/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="41580" yWindow="4520" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
-  <si>
-    <t>#SampleID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Poop1</t>
   </si>
@@ -65,15 +57,6 @@
     <t>PCR_negative</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>PCR water control (water in Tube 5)</t>
-  </si>
-  <si>
-    <t>Mock community (DNA in Tube 4)</t>
-  </si>
-  <si>
     <t>Tissue3</t>
   </si>
   <si>
@@ -83,10 +66,7 @@
     <t>Random2</t>
   </si>
   <si>
-    <t>DNA in 96-well plate</t>
-  </si>
-  <si>
-    <t>DNA extraction blank</t>
+    <t>Sample_ID</t>
   </si>
 </sst>
 </file>
@@ -500,139 +480,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>